<commit_message>
refactor of trade_request pricing, portfolio
</commit_message>
<xml_diff>
--- a/TradeManager/test/test_data/Trade Request Example.xlsx
+++ b/TradeManager/test/test_data/Trade Request Example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>model</t>
   </si>
@@ -63,9 +63,6 @@
     <t>BHYUJ</t>
   </si>
   <si>
-    <t>Almost Cash</t>
-  </si>
-  <si>
     <t>1455-0987</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
   </si>
   <si>
     <t>EMHY</t>
-  </si>
-  <si>
-    <t>LQD</t>
   </si>
   <si>
     <t>EMB</t>
@@ -471,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +481,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -496,13 +490,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,7 +590,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -606,7 +600,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,171 +680,157 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3">
-        <v>10000</v>
+        <v>5687.21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D18" s="3">
-        <v>5687.21</v>
+        <v>750</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="3">
-        <v>750</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
       <c r="D20" s="3">
-        <v>32.5</v>
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>5.36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="3">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E21">
-        <v>5.36</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3">
-        <v>99</v>
-      </c>
-      <c r="E22">
-        <v>100</v>
+        <v>9994.67</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="3">
-        <v>9994.67</v>
+        <v>18</v>
+      </c>
+      <c r="D23">
+        <v>172.09039999999999</v>
+      </c>
+      <c r="E23">
+        <v>50.381</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>172.09039999999999</v>
-      </c>
-      <c r="E24">
-        <v>50.381</v>
+        <v>121.1987</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25">
-        <v>121.1987</v>
+        <v>63.023800000000001</v>
       </c>
       <c r="E25">
-        <v>118.4</v>
+        <v>114.47</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>63.023800000000001</v>
+        <v>126.48399999999999</v>
       </c>
       <c r="E26">
-        <v>114.47</v>
+        <v>106.66</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>126.48399999999999</v>
+        <v>434.28129999999999</v>
       </c>
       <c r="E27">
-        <v>106.66</v>
+        <v>27.03</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D28">
-        <v>434.28129999999999</v>
-      </c>
-      <c r="E28">
-        <v>27.03</v>
+        <v>360.44</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29">
-        <v>360.44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more tests and create more validation methods in RawRequest
</commit_message>
<xml_diff>
--- a/TradeManager/test/test_data/Trade Request Example.xlsx
+++ b/TradeManager/test/test_data/Trade Request Example.xlsx
@@ -24,9 +24,6 @@
     <t>symbol</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
     <t>AGG</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>5268-5955</t>
   </si>
   <si>
-    <t>account</t>
-  </si>
-  <si>
     <t>tsm1500</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>account_cash</t>
+  </si>
+  <si>
+    <t>account_number</t>
+  </si>
+  <si>
+    <t>model_weight</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,22 +481,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>0.15</v>
@@ -516,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>0.1</v>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>0.05</v>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
         <v>0.02</v>
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>0.01</v>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
         <v>0.04</v>
@@ -576,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>0.03</v>
@@ -585,30 +585,30 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
       </c>
       <c r="D11" s="3">
         <v>100</v>
@@ -616,10 +616,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3">
         <v>352</v>
@@ -627,10 +627,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
         <v>98.2</v>
@@ -638,10 +638,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="3">
         <v>74.5</v>
@@ -649,10 +649,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3">
         <v>1000</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3">
         <v>69.5</v>
@@ -677,10 +677,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3">
         <v>5687.21</v>
@@ -688,10 +688,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="3">
         <v>750</v>
@@ -699,10 +699,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="3">
         <v>32.5</v>
@@ -710,10 +710,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
         <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
       </c>
       <c r="D20" s="3">
         <v>67</v>
@@ -724,10 +724,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3">
         <v>99</v>
@@ -738,10 +738,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D22" s="3">
         <v>9994.67</v>
@@ -749,10 +749,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23">
         <v>172.09039999999999</v>
@@ -763,10 +763,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24">
         <v>121.1987</v>
@@ -774,10 +774,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25">
         <v>63.023800000000001</v>
@@ -788,10 +788,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26">
         <v>126.48399999999999</v>
@@ -802,10 +802,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27">
         <v>434.28129999999999</v>
@@ -816,10 +816,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D28">
         <v>360.44</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>